<commit_message>
added dynamic xml runner class
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -9,14 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPageTest1" sheetId="3" r:id="rId2"/>
-    <sheet name="MyFirstTest1" sheetId="4" r:id="rId3"/>
-    <sheet name="LoginPageTest" sheetId="5" r:id="rId4"/>
-    <sheet name="MyFirstTest" sheetId="6" r:id="rId5"/>
+    <sheet name="LoginPageTest" sheetId="5" r:id="rId2"/>
+    <sheet name="MyFirstTest" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -61,9 +59,6 @@
   </si>
   <si>
     <t>Avinash</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>myFirstTestt</t>
@@ -88,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,23 +91,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,18 +107,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -161,55 +135,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,7 +452,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -533,8 +470,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>14</v>
+      <c r="A2" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -542,10 +479,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -554,132 +491,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3"/>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -691,16 +502,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -711,12 +522,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -728,25 +539,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -757,10 +568,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -771,7 +582,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
updating json reading functionality
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -494,7 +494,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -527,7 +529,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed the failed screenshot in report
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160"/>
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Test_Case</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -482,7 +485,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated categories in extent reporting
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>Test_Case</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -485,7 +482,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added method in test base
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24507691-F629-4781-BF5F-33C17176F476}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD043C0-E0B1-44EC-8282-5FB9B72480B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-240" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
   <si>
     <t>TCID</t>
   </si>
@@ -84,6 +84,30 @@
   </si>
   <si>
     <t>validation_message2</t>
+  </si>
+  <si>
+    <t>app_type</t>
+  </si>
+  <si>
+    <t>MobiControl</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>Soti DB</t>
+  </si>
+  <si>
+    <t>TC_375426</t>
+  </si>
+  <si>
+    <t>deleteApplication</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -527,10 +551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C61D4B-1E35-4B2E-A2F2-2072BDFEADA3}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,13 +564,14 @@
     <col min="3" max="3" width="37.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="7" width="14.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="33" style="4" customWidth="1"/>
+    <col min="9" max="9" width="53.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -563,16 +588,22 @@
         <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -588,13 +619,19 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -606,12 +643,114 @@
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -621,6 +760,12 @@
     <hyperlink ref="D2" r:id="rId2" xr:uid="{4DABE741-E756-4DB7-913A-70C241B0CD1B}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{4B256051-81F7-430F-B85B-D2F1E061A55F}"/>
     <hyperlink ref="D3" r:id="rId4" xr:uid="{29EC8ED3-BC95-4A3E-A095-ECBFEF82CB08}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{5CA62D01-93C9-4C42-9A46-934E54FA9E2A}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{CB9C9AB9-FCE8-4519-8377-3D36F7D64245}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{FBFAB3B2-AFB3-4353-81D9-1C05ABC8E3DA}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{1439B88C-626A-4EAC-AE9E-72DAE46B0B03}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{C45386B9-4FF0-4F13-A0D6-FAD0F825AEEF}"/>
+    <hyperlink ref="D6" r:id="rId10" xr:uid="{070D6895-5ED8-4572-A7C7-71A4AF050884}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
checking latest IDP code
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD043C0-E0B1-44EC-8282-5FB9B72480B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C2EFF3-250E-42C9-A0E1-4A3A23F306FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
     <sheet name="R03" sheetId="7" r:id="rId2"/>
+    <sheet name="Tenant_Tests" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="36">
   <si>
     <t>TCID</t>
   </si>
@@ -104,10 +105,34 @@
     <t>deleteApplication</t>
   </si>
   <si>
-    <t>account</t>
-  </si>
-  <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>createUser</t>
+  </si>
+  <si>
+    <t>createTenant</t>
+  </si>
+  <si>
+    <t>http://qa2012r2-kv3.inqa.soti.net/login</t>
+  </si>
+  <si>
+    <t>adminidp@abc.com</t>
+  </si>
+  <si>
+    <t>Tenant_Tests</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>industry_type</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
   </si>
 </sst>
 </file>
@@ -190,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -209,6 +234,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -516,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +570,14 @@
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -626,12 +662,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>6</v>
@@ -658,12 +694,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>6</v>
@@ -695,7 +731,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>6</v>
@@ -724,7 +760,7 @@
     </row>
     <row r="6" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>2</v>
@@ -769,4 +805,113 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC628226-6F23-4A23-BCB8-6ED654FB408C}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{E7FB812B-3BA9-47A9-813A-D6837A744A55}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{06E08B2A-D0DC-48FA-9F9D-591A421B5E49}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{5EA7B01A-5291-45A8-88BD-784F6264F7B4}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{E8ACBA7B-01F8-408F-80D8-41D4FDCC012B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>